<commit_message>
Writing to xlsx and including number of data points
</commit_message>
<xml_diff>
--- a/data/Ethanol.xlsx
+++ b/data/Ethanol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Study Old/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sharpandhowells2015-my.sharepoint.com/personal/lee_sharpandhowells_com_au/Documents/Documents/GitHub/Curve_Optimising/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{825AB22E-D6D8-1947-AB10-846037A12D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{825AB22E-D6D8-1947-AB10-846037A12D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{714E33B5-C1DA-476E-914C-8C6BB66C252E}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{26731E02-B61E-284A-8F48-A390778ACEA0}"/>
+    <workbookView xWindow="30195" yWindow="1395" windowWidth="23850" windowHeight="12735" xr2:uid="{26731E02-B61E-284A-8F48-A390778ACEA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -90,11 +90,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -103,6 +114,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,18 +431,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A75066-CB66-9642-8BFE-B70A2661F8F0}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="10.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0.05</v>
       </c>
@@ -444,7 +458,7 @@
         <v>4.5778267119755071E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>0.1</v>
       </c>
@@ -452,7 +466,7 @@
         <v>8.9213696915770552E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>0.5</v>
       </c>
@@ -460,7 +474,7 @@
         <v>0.4786032245978778</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -468,7 +482,7 @@
         <v>0.99309338643223</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -476,7 +490,7 @@
         <v>3.0586292662265491</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -484,7 +498,7 @@
         <v>4.9779752692950066</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -492,12 +506,28 @@
         <v>6.6991247129700513</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>9.784182525324475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3">
+        <v>14.676</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3">
+        <v>19.399999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Looking at ULOQ/LLOQ Ratios
</commit_message>
<xml_diff>
--- a/data/Ethanol.xlsx
+++ b/data/Ethanol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sharpandhowells2015-my.sharepoint.com/personal/lee_sharpandhowells_com_au/Documents/Documents/GitHub/Curve_Optimising/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{825AB22E-D6D8-1947-AB10-846037A12D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19490311-272D-4BE1-8B7D-BA8328CA2C6E}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{825AB22E-D6D8-1947-AB10-846037A12D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{978C9BCC-98CC-4514-8FB9-994838903E10}"/>
   <bookViews>
-    <workbookView xWindow="30105" yWindow="2700" windowWidth="26535" windowHeight="12405" xr2:uid="{26731E02-B61E-284A-8F48-A390778ACEA0}"/>
+    <workbookView xWindow="30540" yWindow="3135" windowWidth="26535" windowHeight="12405" xr2:uid="{26731E02-B61E-284A-8F48-A390778ACEA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -90,22 +90,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -114,9 +103,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,7 +424,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B9" sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -516,9 +506,11 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>